<commit_message>
the translation of test cases to gherkyn language is carried out
</commit_message>
<xml_diff>
--- a/RepositoryGherkyn/Gherkin.xlsx
+++ b/RepositoryGherkyn/Gherkin.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Estudio\Documents\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Estudio\Documents\QA\petStoreQA\QAProject\RepositoryGherkyn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8760" windowHeight="8748" tabRatio="867" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8760" windowHeight="8748" tabRatio="867" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subirimg" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="376">
   <si>
     <t>Identificador</t>
   </si>
@@ -1077,9 +1077,6 @@
   </si>
   <si>
     <t xml:space="preserve">Actualizar el Status de la mascota ingresando Numeros </t>
-  </si>
-  <si>
-    <t>Actualizar el status de la mascota dejando Vacio</t>
   </si>
   <si>
     <t>Ingresar un String en el Id de la mascota</t>
@@ -1451,33 +1448,6 @@
 * tener parametros del Json
 *Tener mascotas con estado Pending
 </t>
-  </si>
-  <si>
-    <t>1. Ingrese a Postman
-2. Abra una request o peticion
-3. Seleccionar un metodo GET
-4.Ingresa *URL https://petstore.swagger.io/v2/swagger.json
-5. Ingresa el PATH o la URL/pet/{petId}
-6. Complete el siguiente Json:
-{
-  "id": int,
-  "category": {
-    "id": int,
-    "name": "string"
-  },
-  "name": "doggie",
-  "photoUrls": [
-    "string"
-  ],
-  "tags": [
-    {
-      "id": int,
-      "name": "string"
-    }
-  ],
-  "status": "available"
-}
-7.Click en Send Btn.</t>
   </si>
   <si>
     <t>1. Ingrese a Postman
@@ -1559,24 +1529,6 @@
   </si>
   <si>
     <t>Escribir la palabra "Manzana" en el espacio categoy  de la mascota</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feature: Add Pet
-As QA Automation
-I want to Add a pet
-to validate the status code and response
-Backgound: consuming service
- *URL 
-Scenario: Addpet with valid and invalid data
-Given the path  'pet'
-And  method  post
-When the body type params {{id: &lt;id&gt;, category: {id: &lt;id&gt; , name: &lt;name&gt;}, name:&lt;name&gt;, photoUrls:[ &lt;photoUrls&gt;}], tags:[ {id:&lt;id&gt;, name:&lt;name&gt;}] status: &lt;status&gt;}}
-Then status code 201
-And match response &lt;expected&gt;
-Example|:
-id   |categoryid |categoryName |name   |photourls   |tags  |status       |expected                                                                                                               |
-|01   |001             |tux                    | danna | dog.jpj       |dog   |avaible    |{id: 'int', name: 'string', photoUrls: 'string' ,  tags: 'string',  status: 'string' }|
-</t>
   </si>
   <si>
     <t>Escribir un texto en el espacio id Categoria de la mascota</t>
@@ -1673,33 +1625,6 @@
     <t>CP090</t>
   </si>
   <si>
-    <t>1. Ingrese a Postman
-2. Abra una request o peticion
-3. Seleccionar un metodo GET
-4.  Ingresa *URL https://petstore.swagger.io/v2/swagger.json
-5. Ingresa el PATH o la URL/pet/{petId}
-6. Complete el siguiente Json:
-{
-  "id": int,
-  "category": {
-    "id": int,
-    "name": "string"
-  },
-  "name": "string",
-  "photoUrls": [
-    "string"
-  ],
-  "tags": [
-    {
-      "id": int,
-      "name": "string"
-    }
-  ],
-  "status": "available"
-}
-7.Click en Send Btn.</t>
-  </si>
-  <si>
     <t>Si la petición es correcta se debe mostrar status code 200  
 successful operation con la mascota buscada
 {
@@ -1722,21 +1647,190 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature: update a pet
+    <t>1. Ingrese a Postman
+2. Abra una request o peticion
+3. Seleccionar un metodo GET
+4.  Ingresa *URL https://petstore.swagger.io/v2/swagger.json
+5. Ingresa el PATH   {petId}
+6. Dar click en Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Ingrese a Postman
+2. Abra una request o peticion
+3. Seleccionar un metodo GET
+4.  Ingresa *URL https://petstore.swagger.io/v2/swagger.json
+5.Ingresa el PATH /pet/{petId}
+6. Ir a la pestaña Headers
+7. seleccionar X-api-Key
+8. ingesar un valor en el espacio Value
+9.Click en Send Btn.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature: Add Pet
+As QA Automation
+I want to Add a pet
+to validate the status code and response
+Backgound: consuming service
+ *URL 
+Scenario: Addpet with valid and invalid data
+Given the path  'pet'
+When  method  post
+Then status code 201
+And match response ==
+{
+  "id": int ,
+  "category": {
+    "id": int,
+    "name": "string"
+  },
+  "name": "string",
+  "photoUrls": [
+    "string"
+  ],
+  "tags": [
+    {
+      "id": int,
+      "name": "string"
+    }
+  ],
+  "status": "string"
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature: filter pet by id
+As QA Automation
+I want to filter pet by id
+to validate the status code and response
+Backgound: consuming service
+ *URL 
+Scenario: filter pet by id and validate data
+Given the path   &lt;petId&gt;
+When  method  get
+Then status code 200
+And match response ==
+{
+  "id": int,
+  "category": {
+    "id": int,
+    "name": "string"
+  },
+  "name": "string",
+  "photoUrls": [
+    "string"
+  ],
+  "tags": [
+    {
+      "id": int,
+      "name": "string"
+    }
+  ],
+  "status": "available"
+}
+</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature: filter pet by other id
+As QA Automation
+I want to filter pet by id and validate is true 
+to validate the status code and response
+Backgound: consuming service
+ *URL 
+Scenario Outline: filter pet by id and invalidate data
+Given the path   &lt;tId&gt;
+When  method  get
+Then status code 404
+And match response &lt;expends&gt;
+Examples:
+|id              | expends |
+|0,0            | {"code": 1, "type": "error", "message": "Pet not found"} |
+| ads          | {"code": 1, "type": "error", "message": "Pet not found"} |
+|                   | {"code": 1, "type": "error", "message": "Pet not found"} |
+|8979879  | {"code": 1, "type": "error", "message": "Pet not found"} |
+|adsijeopw89*/olpedolertoeld          | {"code": 1, "type": "error", "message": "Pet not found"} |
+</t>
+  </si>
+  <si>
+    <t>Feature: update a pet
 As QA Automation
 I want to update a pet
 to validate the status code and response
 Backgound: consuming service
  *URL 
-Scenario:  update a pet with a data
+Scenario Outline:  update a pet with a data
 Given the path  'pet'
 And  method  put
 When the body type params {{id: &lt;id&gt;, category: {id: &lt;id&gt; , name: &lt;name&gt;}, name:&lt;name&gt;, photoUrls:[ &lt;photoUrls&gt;}], tags:[ {id:&lt;id&gt;, name:&lt;name&gt;}] status: &lt;status&gt;}}
 Then status code 200
-And match response &lt;expected&gt;
-Example|:
-id   |categoryid |categoryName |name   |photourls   |tags  |status       |expected                                                                                                               |
-|01   |001             |tux                    | danna | dog.jpj       |dog   |avaible    |{id: 'int', name: 'string', photoUrls: 'string' ,  tags: 'string',  status: 'string' }|
+And match response == expect
+|id    |categoryid           |categoryName    |name           |photourls    |tags     |status    |expected        |
+|001 |001                      | danna                   | dog              |dogy.jpg       |dog     |avaible    |{"id":int, "category": { "id": int,  "name": "string" }, "name": "doggie", "photoUrls": [    "string" ],"tags": [{"id": 0, "name": "string"}],  "status": "available"}
+|001 |001                      | danna                   | dog              |dog.jpg       |dog     |avaible    |{"id":int, "category": { "id": int,  "name": "string" }, "name": "doggie", "photoUrls": [    "string" ],"tags": [{"id": 0, "name": "string"}],  "status": "available"}
+|001 |001                      | danna                   | dog              |dog.jpg       |dog     |pending    |{"id":int, "category": { "id": int,  "name": "string" }, "name": "doggie", "photoUrls": [    "string" ],"tags": [{"id": 0, "name": "string"}],  "status": "available"}
+|001 |001                      | danna                   | dog              |dog.jpg       |dog     |sold    |{"id":int, "category": { "id": int,  "name": "string" }, "name": "doggie", "photoUrls": [    "string" ],"tags": [{"id": 0, "name": "string"}],  "status": "available"}</t>
+  </si>
+  <si>
+    <t>Actualizar el status de la mascota dejando Vacio el espacio de status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature: update a pet with status code fail
+As QA Automation
+I want to update a pet
+to validate the status code
+Backgound: consuming service
+ *URL 
+Scenario Outline:  update a pet with wrong data 
+Given the path  'pet'
+And  method  put
+When the body type params {{id: &lt;id&gt;, category: {id: &lt;id&gt; , name: &lt;name&gt;}, name:&lt;name&gt;, photoUrls:[ &lt;photoUrls&gt;}], tags:[ {id:&lt;id&gt;, name:&lt;name&gt;}] status: &lt;status&gt;}}
+Then status &lt;code&gt;
+|id    |categoryid           |categoryName    |name           |photourls    |tagsid|tagasname     |status        |code      |
+|001 |001                      | danna                   | dog              |dogy.jpg  |01      |dog     |***//    |400 |
+|001 |001                      | danna                   | dog              |dog.jpg       |01|dog     |avaiblepolirdteprosloprd  |400|
+|001 |001                      | danna                   | dog              |dog.jpg       |01|dog     |154896   | 400|
+|001 |001                      | danna                   | dog              |dog.jpg       |01|dog     |free    |400|
+|001 |001                      | danna                   | dog              |dog.jpg       |01|dog     |         |400|
+|abc  |001                      | danna                   | dog              |dogy.jpg     |01  |dog     |avaible   |400 |
+|/*/* |001                      | danna                   | dog              |dogy.jpg       |01  |dog     |avaible   |400 |
+|     |001                      | danna                   | dog              |dogy.jpg       |01   |dog     |avaible   |400 |
+|ade001ertyhfescefasedgbhrxc |001                      | danna                    |01| dog              |dogy.jpg       |dog     |avaible   |400 |
+|0.01 |001                      | danna                   | dog              |dogy.jpg    |01   |dog     |avaible   |400 |
+|001 |/*+-                     | danna                   | dog              |dogy.jpg       |01  |dog     |avaible   |400 |
+|001 |adosdp                     | danna                   | dog              |dogy.jpg  |01     |dog     |avaible   |400 |
+|001 |ad001sdoepdiekodlasodiepdad  | danna                   | dog              |01  |dogy.jpg       |dog     |avaible   |400 |
+|001 |                       | danna                   | dog              |dogy.jpg          |01|dog     |avaible   |400 |
+|001 |001                      | 1848                  | dog              |dogy.jpg        |01|dog     |avaible   |400 |
+|001 |001                      |                         | dog              |dogy.jpg          |01 |dog     |avaible   |400 |
+|001 |001                      | danna*/8                   | dog              |dogy.jpg  |01     |dog     |avaible   |400 |
+|001 |001                      | dannaaspeod878dasdeijdiedasbdj                   |01  | dog              |dogy.jpg       |dog     |avaible   |400 |
+|001 |001                      | danna                   | manzana              |dogy.jpg |01      |dog     |avaible   |400 |
+|001 |001                      | danna                   | 121545             |dogy.jpg      |01 |dog     |avaible   |400 |
+|001 |001                      | danna                   |                  |dogy.jpg            |01|dog     |avaible   |400 |
+|001 |001                      | danna                   | dogspñeorikeodpaospekdieopaso  |dogy.jpg     |01  |dog     |avaible   |400 |
+|001 |001                      | danna                   | /*-+-           |dogy.jpg       |01|dog     |avaible   |400 |
+|001 |001                      | danna                   | 4858             |dogy.jpg       |01|dog     |avaible   |400 |
+|001 |001                      | danna                   | danna              |dogy.jpg      |01 |dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.mp4       |01|dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.pdf       |01 |dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |                   |01 |dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogyjpg       |01 |dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |1458           |01  |dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01 |peras     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01  |/*-+    |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01  |dogopelidopeirkeospñasorfsed |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01  |      |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01 |dogpeodpasodepda´dedpoad |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |    |dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |spoeldoepdolepodpeladpods |dog     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01  |dogoepdoepdlasodeodamdadmsdmeo     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01  |78545     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01  |d*/*--     |avaible    |400 |
+|001 |001                      | danna                   | dog              |dogy.jpg       |01  |     |avaible    |400 |
 </t>
   </si>
   <si>
@@ -1747,32 +1841,33 @@
 Backgound: consuming service
  *URL 
 Scenario:  update a pet with a data
-Given the path  'pet,'petid'
-And  method delete
-When the body type params {{id: &lt;id&gt;, category: {id: &lt;id&gt; , name: &lt;name&gt;}, name:&lt;name&gt;, photoUrls:[ &lt;photoUrls&gt;}], tags:[ {id:&lt;id&gt;, name:&lt;name&gt;}] status: &lt;status&gt;}}
+Given the path  'pet, 'petid'
+When  method delete
 Then status code 200
-And match response &lt;expected&gt;
-Example|:
-id   |categoryid |categoryName |name   |photourls   |tags  |status       |expected                                                              |                                                                                                        
-|01   |001             |tux                    | danna | dog.jpj       |dog   |avaible    |{'code': '200', 'type':'unknown', 'message':'1'}|
+And match response == 
+{
+  "code": 200,
+  "type": "unknown",
+  "message": "1"
+}}|
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Feature: filter pet by id
+    <t xml:space="preserve">Feature:  Delete a pet with invalid ID
 As QA Automation
-I want to filter pet by id
-to validate the status code and response
+I want to delete a pet
+to validate the status code
 Backgound: consuming service
  *URL 
-Scenario: filter pet by id and validate data
-Given the path  'pet', petId'
-And  method  get
-When the body type params {{id: &lt;id&gt;, category: {id: &lt;id&gt; , name: &lt;name&gt;}, name:&lt;name&gt;, photoUrls:[ &lt;photoUrls&gt;}], tags:[ {id:&lt;id&gt;, name:&lt;name&gt;}] status: &lt;status&gt;}}
-Then status code 200
-And match response &lt;expected&gt;
-Example|:
-id   |categoryid |categoryName |name   |photourls   |tags  |status       |expected                                                                                                               |
-|01   |001             |tux                    | danna | dog.jpj       |dog   |avaible    |{id: 'int', name: 'string', photoUrls: 'string' ,  tags: 'string',  status: 'string' }|
+Scenario:  update a pet with invalid Id
+Given the path  'pet, &lt;petid&gt;
+When  method delete
+Then status code 400
+|Petid      |code |
+|001         |400||
+|00.1 |      |400|
+|             | 400|
+|abc       |400 |
 </t>
   </si>
 </sst>
@@ -2000,7 +2095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2161,6 +2256,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3217,7 +3324,7 @@
         <v>94</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>95</v>
@@ -32408,8 +32515,8 @@
   </sheetPr>
   <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="H18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -32486,7 +32593,7 @@
         <v>7</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
@@ -32518,13 +32625,13 @@
         <v>131</v>
       </c>
       <c r="E5" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F5" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="F5" s="36" t="s">
-        <v>335</v>
-      </c>
       <c r="G5" s="36" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H5" s="37" t="s">
         <v>17</v>
@@ -32533,7 +32640,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>350</v>
+        <v>367</v>
       </c>
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
@@ -32565,13 +32672,13 @@
         <v>133</v>
       </c>
       <c r="E6" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="F6" s="36" t="s">
-        <v>335</v>
-      </c>
       <c r="G6" s="41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H6" s="42" t="s">
         <v>17</v>
@@ -32580,7 +32687,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="60" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="K6" s="33"/>
       <c r="L6" s="33"/>
@@ -32612,10 +32719,10 @@
         <v>169</v>
       </c>
       <c r="E7" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F7" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>22</v>
@@ -32654,13 +32761,13 @@
         <v>135</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E8" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F8" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>22</v>
@@ -32699,13 +32806,13 @@
         <v>134</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E9" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F9" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>22</v>
@@ -32747,10 +32854,10 @@
         <v>137</v>
       </c>
       <c r="E10" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F10" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G10" s="41" t="s">
         <v>22</v>
@@ -32792,10 +32899,10 @@
         <v>139</v>
       </c>
       <c r="E11" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G11" s="41" t="s">
         <v>22</v>
@@ -32837,10 +32944,10 @@
         <v>141</v>
       </c>
       <c r="E12" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F12" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G12" s="41" t="s">
         <v>22</v>
@@ -32882,10 +32989,10 @@
         <v>144</v>
       </c>
       <c r="E13" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G13" s="41" t="s">
         <v>22</v>
@@ -32927,10 +33034,10 @@
         <v>145</v>
       </c>
       <c r="E14" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F14" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G14" s="41" t="s">
         <v>22</v>
@@ -32972,10 +33079,10 @@
         <v>147</v>
       </c>
       <c r="E15" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F15" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G15" s="41" t="s">
         <v>22</v>
@@ -33017,10 +33124,10 @@
         <v>170</v>
       </c>
       <c r="E16" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F16" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G16" s="41" t="s">
         <v>22</v>
@@ -33062,10 +33169,10 @@
         <v>149</v>
       </c>
       <c r="E17" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F17" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G17" s="41" t="s">
         <v>22</v>
@@ -33107,10 +33214,10 @@
         <v>171</v>
       </c>
       <c r="E18" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F18" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G18" s="41" t="s">
         <v>22</v>
@@ -33152,10 +33259,10 @@
         <v>151</v>
       </c>
       <c r="E19" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G19" s="41" t="s">
         <v>22</v>
@@ -33190,16 +33297,16 @@
         <v>70</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E20" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F20" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G20" s="41" t="s">
         <v>22</v>
@@ -33223,10 +33330,10 @@
         <v>172</v>
       </c>
       <c r="E21" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F21" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G21" s="41" t="s">
         <v>22</v>
@@ -33250,10 +33357,10 @@
         <v>173</v>
       </c>
       <c r="E22" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F22" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G22" s="41" t="s">
         <v>22</v>
@@ -33271,16 +33378,16 @@
         <v>74</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E23" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F23" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G23" s="41" t="s">
         <v>22</v>
@@ -33298,16 +33405,16 @@
         <v>75</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E24" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F24" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G24" s="41" t="s">
         <v>22</v>
@@ -33331,10 +33438,10 @@
         <v>174</v>
       </c>
       <c r="E25" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F25" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G25" s="41" t="s">
         <v>22</v>
@@ -33358,10 +33465,10 @@
         <v>175</v>
       </c>
       <c r="E26" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F26" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G26" s="41" t="s">
         <v>22</v>
@@ -33385,10 +33492,10 @@
         <v>176</v>
       </c>
       <c r="E27" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F27" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F27" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G27" s="41" t="s">
         <v>22</v>
@@ -33412,10 +33519,10 @@
         <v>177</v>
       </c>
       <c r="E28" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F28" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G28" s="41" t="s">
         <v>22</v>
@@ -33439,10 +33546,10 @@
         <v>178</v>
       </c>
       <c r="E29" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F29" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F29" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G29" s="41" t="s">
         <v>22</v>
@@ -33466,10 +33573,10 @@
         <v>179</v>
       </c>
       <c r="E30" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F30" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="G30" s="41" t="s">
         <v>22</v>
@@ -33558,8 +33665,8 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="D8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -33569,7 +33676,7 @@
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="21.77734375" customWidth="1"/>
     <col min="6" max="6" width="33.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" customWidth="1"/>
     <col min="9" max="9" width="9.33203125" customWidth="1"/>
     <col min="10" max="10" width="107.5546875" customWidth="1"/>
@@ -33635,7 +33742,7 @@
         <v>7</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
@@ -33655,10 +33762,10 @@
       <c r="Z5" s="19"/>
       <c r="AA5" s="19"/>
     </row>
-    <row r="6" spans="1:27" s="54" customFormat="1" ht="265.2">
+    <row r="6" spans="1:27" s="54" customFormat="1" ht="357">
       <c r="A6" s="50"/>
       <c r="B6" s="51" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>34</v>
@@ -33667,13 +33774,13 @@
         <v>182</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="H6" s="53" t="s">
         <v>17</v>
@@ -33682,7 +33789,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="48" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="K6" s="50"/>
       <c r="L6" s="50"/>
@@ -33702,10 +33809,10 @@
       <c r="Z6" s="50"/>
       <c r="AA6" s="50"/>
     </row>
-    <row r="7" spans="1:27" s="54" customFormat="1" ht="100.2" customHeight="1">
+    <row r="7" spans="1:27" s="54" customFormat="1" ht="181.2" customHeight="1">
       <c r="A7" s="50"/>
       <c r="B7" s="51" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C7" s="52" t="s">
         <v>183</v>
@@ -33714,10 +33821,10 @@
         <v>184</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="G7" s="53" t="s">
         <v>185</v>
@@ -33728,8 +33835,12 @@
       <c r="I7" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
+      <c r="J7" s="61" t="s">
+        <v>370</v>
+      </c>
+      <c r="K7" s="50" t="s">
+        <v>369</v>
+      </c>
       <c r="L7" s="50"/>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
@@ -33747,9 +33858,9 @@
       <c r="Z7" s="50"/>
       <c r="AA7" s="50"/>
     </row>
-    <row r="8" spans="1:27" s="54" customFormat="1" ht="265.2">
+    <row r="8" spans="1:27" s="54" customFormat="1" ht="81.599999999999994">
       <c r="B8" s="51" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>186</v>
@@ -33758,10 +33869,10 @@
         <v>187</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="G8" s="53" t="s">
         <v>185</v>
@@ -33772,10 +33883,11 @@
       <c r="I8" s="53" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" s="54" customFormat="1" ht="265.2">
+      <c r="J8" s="61"/>
+    </row>
+    <row r="9" spans="1:27" s="54" customFormat="1" ht="81.599999999999994">
       <c r="B9" s="51" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C9" s="52" t="s">
         <v>188</v>
@@ -33784,10 +33896,10 @@
         <v>73</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F9" s="53" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="G9" s="53" t="s">
         <v>185</v>
@@ -33798,8 +33910,9 @@
       <c r="I9" s="53" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" s="54" customFormat="1" ht="265.2">
+      <c r="J9" s="61"/>
+    </row>
+    <row r="10" spans="1:27" s="54" customFormat="1" ht="81.599999999999994">
       <c r="B10" s="51" t="s">
         <v>180</v>
       </c>
@@ -33810,10 +33923,10 @@
         <v>191</v>
       </c>
       <c r="E10" s="49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="G10" s="53" t="s">
         <v>185</v>
@@ -33824,8 +33937,9 @@
       <c r="I10" s="53" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" s="54" customFormat="1" ht="265.2">
+      <c r="J10" s="61"/>
+    </row>
+    <row r="11" spans="1:27" s="54" customFormat="1" ht="71.400000000000006">
       <c r="B11" s="51" t="s">
         <v>181</v>
       </c>
@@ -33836,10 +33950,10 @@
         <v>192</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="G11" s="53" t="s">
         <v>193</v>
@@ -33850,8 +33964,12 @@
       <c r="I11" s="53" t="s">
         <v>24</v>
       </c>
+      <c r="J11" s="61"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J7:J11"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="I5:I11">
       <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
@@ -33873,8 +33991,8 @@
   </sheetPr>
   <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -33887,7 +34005,7 @@
     <col min="6" max="6" width="33.44140625" customWidth="1"/>
     <col min="7" max="7" width="21.21875" customWidth="1"/>
     <col min="8" max="8" width="19.44140625" customWidth="1"/>
-    <col min="10" max="10" width="93" customWidth="1"/>
+    <col min="10" max="10" width="148.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="25.2">
@@ -33950,7 +34068,7 @@
         <v>7</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
@@ -33973,7 +34091,7 @@
     <row r="5" spans="1:27" s="39" customFormat="1" ht="246" customHeight="1">
       <c r="A5" s="33"/>
       <c r="B5" s="42" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>200</v>
@@ -33982,10 +34100,10 @@
         <v>201</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G5" s="41" t="s">
         <v>202</v>
@@ -33996,8 +34114,8 @@
       <c r="I5" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="48" t="s">
-        <v>369</v>
+      <c r="J5" s="60" t="s">
+        <v>371</v>
       </c>
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
@@ -34020,7 +34138,7 @@
     <row r="6" spans="1:27" s="39" customFormat="1" ht="195" customHeight="1">
       <c r="A6" s="33"/>
       <c r="B6" s="42" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>203</v>
@@ -34029,10 +34147,10 @@
         <v>206</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G6" s="41" t="s">
         <v>202</v>
@@ -34043,7 +34161,7 @@
       <c r="I6" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="33"/>
+      <c r="J6" s="60"/>
       <c r="K6" s="33"/>
       <c r="L6" s="33"/>
       <c r="M6" s="33"/>
@@ -34065,7 +34183,7 @@
     <row r="7" spans="1:27" s="39" customFormat="1" ht="196.2" customHeight="1">
       <c r="A7" s="33"/>
       <c r="B7" s="42" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>204</v>
@@ -34074,10 +34192,10 @@
         <v>207</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>202</v>
@@ -34088,7 +34206,7 @@
       <c r="I7" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="33"/>
+      <c r="J7" s="60"/>
       <c r="K7" s="33"/>
       <c r="L7" s="33"/>
       <c r="M7" s="33"/>
@@ -34110,7 +34228,7 @@
     <row r="8" spans="1:27" s="39" customFormat="1" ht="192.6" customHeight="1">
       <c r="A8" s="33"/>
       <c r="B8" s="42" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C8" s="40" t="s">
         <v>205</v>
@@ -34119,10 +34237,10 @@
         <v>208</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>202</v>
@@ -34133,7 +34251,7 @@
       <c r="I8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="33"/>
+      <c r="J8" s="60"/>
       <c r="K8" s="33"/>
       <c r="L8" s="33"/>
       <c r="M8" s="33"/>
@@ -34164,10 +34282,10 @@
         <v>238</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>211</v>
@@ -34178,7 +34296,9 @@
       <c r="I9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="33"/>
+      <c r="J9" s="60" t="s">
+        <v>373</v>
+      </c>
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
       <c r="M9" s="33"/>
@@ -34209,10 +34329,10 @@
         <v>239</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G10" s="41" t="s">
         <v>211</v>
@@ -34223,7 +34343,7 @@
       <c r="I10" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="33"/>
+      <c r="J10" s="62"/>
       <c r="K10" s="33"/>
       <c r="L10" s="33"/>
       <c r="M10" s="33"/>
@@ -34254,10 +34374,10 @@
         <v>241</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G11" s="41" t="s">
         <v>211</v>
@@ -34268,7 +34388,7 @@
       <c r="I11" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="33"/>
+      <c r="J11" s="62"/>
       <c r="K11" s="33"/>
       <c r="L11" s="33"/>
       <c r="M11" s="33"/>
@@ -34299,10 +34419,10 @@
         <v>240</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G12" s="41" t="s">
         <v>211</v>
@@ -34313,7 +34433,7 @@
       <c r="I12" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="33"/>
+      <c r="J12" s="62"/>
       <c r="K12" s="33"/>
       <c r="L12" s="33"/>
       <c r="M12" s="33"/>
@@ -34341,13 +34461,13 @@
         <v>222</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>242</v>
+        <v>372</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G13" s="41" t="s">
         <v>211</v>
@@ -34358,7 +34478,7 @@
       <c r="I13" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="33"/>
+      <c r="J13" s="62"/>
       <c r="K13" s="33"/>
       <c r="L13" s="33"/>
       <c r="M13" s="33"/>
@@ -34383,16 +34503,16 @@
         <v>199</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D14" s="57" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G14" s="41" t="s">
         <v>211</v>
@@ -34403,7 +34523,7 @@
       <c r="I14" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="33"/>
+      <c r="J14" s="62"/>
       <c r="K14" s="33"/>
       <c r="L14" s="33"/>
       <c r="M14" s="33"/>
@@ -34428,16 +34548,16 @@
         <v>216</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G15" s="41" t="s">
         <v>211</v>
@@ -34448,7 +34568,7 @@
       <c r="I15" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="33"/>
+      <c r="J15" s="62"/>
       <c r="K15" s="33"/>
       <c r="L15" s="33"/>
       <c r="M15" s="33"/>
@@ -34473,16 +34593,16 @@
         <v>217</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G16" s="41" t="s">
         <v>211</v>
@@ -34493,7 +34613,7 @@
       <c r="I16" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="33"/>
+      <c r="J16" s="62"/>
       <c r="K16" s="33"/>
       <c r="L16" s="33"/>
       <c r="M16" s="33"/>
@@ -34518,16 +34638,16 @@
         <v>218</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D17" s="57" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G17" s="41" t="s">
         <v>211</v>
@@ -34538,7 +34658,7 @@
       <c r="I17" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="33"/>
+      <c r="J17" s="62"/>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
       <c r="M17" s="33"/>
@@ -34563,16 +34683,16 @@
         <v>219</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G18" s="41" t="s">
         <v>211</v>
@@ -34583,7 +34703,7 @@
       <c r="I18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="33"/>
+      <c r="J18" s="62"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -34608,16 +34728,16 @@
         <v>220</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E19" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G19" s="41" t="s">
         <v>211</v>
@@ -34628,7 +34748,7 @@
       <c r="I19" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="33"/>
+      <c r="J19" s="62"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
       <c r="M19" s="33"/>
@@ -34653,16 +34773,16 @@
         <v>221</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G20" s="41" t="s">
         <v>211</v>
@@ -34673,7 +34793,7 @@
       <c r="I20" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="33"/>
+      <c r="J20" s="62"/>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
@@ -34698,16 +34818,16 @@
         <v>227</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D21" s="57" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G21" s="41" t="s">
         <v>211</v>
@@ -34718,7 +34838,7 @@
       <c r="I21" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="33"/>
+      <c r="J21" s="62"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -34743,16 +34863,16 @@
         <v>228</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G22" s="41" t="s">
         <v>211</v>
@@ -34763,7 +34883,7 @@
       <c r="I22" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="33"/>
+      <c r="J22" s="62"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
       <c r="M22" s="33"/>
@@ -34793,10 +34913,10 @@
         <v>210</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G23" s="41" t="s">
         <v>211</v>
@@ -34807,6 +34927,7 @@
       <c r="I23" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J23" s="62"/>
     </row>
     <row r="24" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B24" s="42" t="s">
@@ -34819,10 +34940,10 @@
         <v>213</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G24" s="41" t="s">
         <v>211</v>
@@ -34833,6 +34954,7 @@
       <c r="I24" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J24" s="62"/>
     </row>
     <row r="25" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B25" s="42" t="s">
@@ -34845,10 +34967,10 @@
         <v>215</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G25" s="41" t="s">
         <v>211</v>
@@ -34859,22 +34981,23 @@
       <c r="I25" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J25" s="62"/>
     </row>
     <row r="26" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B26" s="42" t="s">
         <v>232</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D26" s="59" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E26" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G26" s="41" t="s">
         <v>211</v>
@@ -34885,22 +35008,23 @@
       <c r="I26" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J26" s="62"/>
     </row>
     <row r="27" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B27" s="42" t="s">
         <v>233</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D27" s="59" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G27" s="41" t="s">
         <v>211</v>
@@ -34911,22 +35035,23 @@
       <c r="I27" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J27" s="62"/>
     </row>
     <row r="28" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B28" s="42" t="s">
         <v>234</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D28" s="59" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E28" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G28" s="41" t="s">
         <v>211</v>
@@ -34937,22 +35062,23 @@
       <c r="I28" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J28" s="62"/>
     </row>
     <row r="29" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B29" s="42" t="s">
         <v>235</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D29" s="59" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E29" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G29" s="41" t="s">
         <v>211</v>
@@ -34963,22 +35089,23 @@
       <c r="I29" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J29" s="62"/>
     </row>
     <row r="30" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B30" s="42" t="s">
         <v>236</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D30" s="59" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G30" s="41" t="s">
         <v>211</v>
@@ -34989,22 +35116,23 @@
       <c r="I30" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J30" s="62"/>
     </row>
     <row r="31" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B31" s="42" t="s">
         <v>237</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D31" s="59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G31" s="41" t="s">
         <v>211</v>
@@ -35015,22 +35143,23 @@
       <c r="I31" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J31" s="62"/>
     </row>
     <row r="32" spans="1:27" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B32" s="42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D32" s="59" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E32" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F32" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G32" s="41" t="s">
         <v>211</v>
@@ -35041,22 +35170,23 @@
       <c r="I32" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J32" s="62"/>
+    </row>
+    <row r="33" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B33" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D33" s="59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E33" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F33" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G33" s="41" t="s">
         <v>211</v>
@@ -35067,22 +35197,23 @@
       <c r="I33" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J33" s="62"/>
+    </row>
+    <row r="34" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B34" s="42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D34" s="59" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E34" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G34" s="41" t="s">
         <v>211</v>
@@ -35093,22 +35224,23 @@
       <c r="I34" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J34" s="62"/>
+    </row>
+    <row r="35" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B35" s="42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D35" s="59" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E35" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F35" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G35" s="41" t="s">
         <v>211</v>
@@ -35119,22 +35251,23 @@
       <c r="I35" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J35" s="62"/>
+    </row>
+    <row r="36" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B36" s="42" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D36" s="59" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G36" s="41" t="s">
         <v>211</v>
@@ -35145,22 +35278,23 @@
       <c r="I36" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J36" s="62"/>
+    </row>
+    <row r="37" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B37" s="42" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D37" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E37" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G37" s="41" t="s">
         <v>211</v>
@@ -35171,22 +35305,23 @@
       <c r="I37" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J37" s="62"/>
+    </row>
+    <row r="38" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B38" s="42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D38" s="59" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E38" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G38" s="41" t="s">
         <v>211</v>
@@ -35197,22 +35332,23 @@
       <c r="I38" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J38" s="62"/>
+    </row>
+    <row r="39" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B39" s="42" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D39" s="59" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G39" s="41" t="s">
         <v>211</v>
@@ -35223,22 +35359,23 @@
       <c r="I39" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J39" s="62"/>
+    </row>
+    <row r="40" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B40" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D40" s="59" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F40" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G40" s="41" t="s">
         <v>211</v>
@@ -35249,22 +35386,23 @@
       <c r="I40" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J40" s="62"/>
+    </row>
+    <row r="41" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B41" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C41" s="58" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D41" s="59" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F41" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G41" s="41" t="s">
         <v>211</v>
@@ -35275,22 +35413,23 @@
       <c r="I41" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J41" s="62"/>
+    </row>
+    <row r="42" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B42" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="C42" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="C42" s="58" t="s">
-        <v>279</v>
-      </c>
       <c r="D42" s="59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G42" s="41" t="s">
         <v>211</v>
@@ -35301,22 +35440,23 @@
       <c r="I42" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="43" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J42" s="62"/>
+    </row>
+    <row r="43" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B43" s="42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D43" s="59" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G43" s="41" t="s">
         <v>211</v>
@@ -35327,22 +35467,23 @@
       <c r="I43" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="44" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J43" s="62"/>
+    </row>
+    <row r="44" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B44" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D44" s="59" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G44" s="41" t="s">
         <v>211</v>
@@ -35353,22 +35494,23 @@
       <c r="I44" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J44" s="62"/>
+    </row>
+    <row r="45" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B45" s="42" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D45" s="59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G45" s="41" t="s">
         <v>211</v>
@@ -35379,22 +35521,23 @@
       <c r="I45" s="42" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="2:9" s="39" customFormat="1" ht="285.60000000000002">
+      <c r="J45" s="62"/>
+    </row>
+    <row r="46" spans="2:10" s="39" customFormat="1" ht="285.60000000000002">
       <c r="B46" s="42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C46" s="58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D46" s="59" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E46" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G46" s="41" t="s">
         <v>211</v>
@@ -35405,17 +35548,23 @@
       <c r="I46" s="42" t="s">
         <v>24</v>
       </c>
+      <c r="J46" s="62"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J5:J8"/>
+    <mergeCell ref="J9:J46"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="I4:I46">
       <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -35427,8 +35576,8 @@
   </sheetPr>
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -35501,7 +35650,7 @@
         <v>7</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
@@ -35524,22 +35673,22 @@
     <row r="5" spans="1:27" ht="249" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="30" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>321</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>345</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>322</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>17</v>
@@ -35548,7 +35697,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -35571,19 +35720,19 @@
     <row r="6" spans="1:27" ht="132" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>327</v>
-      </c>
       <c r="E6" s="36" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>36</v>
@@ -35594,7 +35743,9 @@
       <c r="I6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="63" t="s">
+        <v>375</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -35615,22 +35766,22 @@
     </row>
     <row r="7" spans="1:27" ht="184.8">
       <c r="B7" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>324</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>345</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>325</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>17</v>
@@ -35638,25 +35789,26 @@
       <c r="I7" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="J7" s="64"/>
     </row>
     <row r="8" spans="1:27" ht="184.8">
       <c r="B8" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>329</v>
-      </c>
       <c r="E8" s="36" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>17</v>
@@ -35664,25 +35816,26 @@
       <c r="I8" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="J8" s="64"/>
     </row>
     <row r="9" spans="1:27" ht="184.8">
       <c r="B9" s="12" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>331</v>
-      </c>
       <c r="E9" s="36" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>17</v>
@@ -35690,8 +35843,12 @@
       <c r="I9" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="J9" s="64"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J6:J9"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="I4:I9">
       <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
@@ -35788,10 +35945,10 @@
         <v>7</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
@@ -35823,7 +35980,7 @@
         <v>91</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>35</v>
@@ -35869,7 +36026,7 @@
         <v>89</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>90</v>
@@ -35914,7 +36071,7 @@
         <v>77</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>78</v>
@@ -35944,7 +36101,7 @@
         <v>80</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>82</v>
@@ -35974,7 +36131,7 @@
         <v>85</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>86</v>
@@ -36005,7 +36162,7 @@
         <v>92</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
the test case in Gherkyn is modified and the karate repository is started
</commit_message>
<xml_diff>
--- a/RepositoryGherkyn/Gherkin.xlsx
+++ b/RepositoryGherkyn/Gherkin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8760" windowHeight="8748" tabRatio="867" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8760" windowHeight="8748" tabRatio="867" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subirimg" sheetId="1" r:id="rId1"/>
@@ -2276,16 +2276,6 @@
   <dxfs count="8">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -2391,6 +2381,16 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2928,7 +2928,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="E1:F3" totalsRowShown="0">
   <autoFilter ref="E1:F3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="6"/>
+    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="5"/>
     <tableColumn id="2" name="Pet Store Automatizaciones QA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2939,7 +2939,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla135" displayName="Tabla135" ref="E1:F3" totalsRowShown="0">
   <autoFilter ref="E1:F3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="5"/>
+    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="4"/>
     <tableColumn id="2" name="Pet Store Automatizaciones QA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2950,7 +2950,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla1367" displayName="Tabla1367" ref="E1:F3" totalsRowShown="0">
   <autoFilter ref="E1:F3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="4"/>
+    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="3"/>
     <tableColumn id="2" name="Pet Store Automatizaciones QA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2961,7 +2961,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla13678" displayName="Tabla13678" ref="E1:F3" totalsRowShown="0">
   <autoFilter ref="E1:F3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="3"/>
+    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="2"/>
     <tableColumn id="2" name="Pet Store Automatizaciones QA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2972,7 +2972,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla134" displayName="Tabla134" ref="E1:F3" totalsRowShown="0">
   <autoFilter ref="E1:F3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="2"/>
+    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="1"/>
     <tableColumn id="2" name="Pet Store Automatizaciones QA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2983,7 +2983,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla136" displayName="Tabla136" ref="E1:F3" totalsRowShown="0">
   <autoFilter ref="E1:F3"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="1"/>
+    <tableColumn id="1" name="Nombre del Proyecto:" dataDxfId="0"/>
     <tableColumn id="2" name="Pet Store Automatizaciones QA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -32515,8 +32515,8 @@
   </sheetPr>
   <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView topLeftCell="H18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J30"/>
+    <sheetView topLeftCell="G4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -33642,7 +33642,7 @@
     <mergeCell ref="J6:J30"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B30">
-    <cfRule type="uniqueValues" dxfId="0" priority="5"/>
+    <cfRule type="uniqueValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="I4:I30">
@@ -33665,7 +33665,7 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView topLeftCell="D8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -33991,8 +33991,8 @@
   </sheetPr>
   <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -35576,7 +35576,7 @@
   </sheetPr>
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="J6" sqref="J6:J9"/>
     </sheetView>
   </sheetViews>
@@ -36200,7 +36200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>